<commit_message>
Added Aperture (Daylight Threshold)
Found a couple of bits in the non-volatile storage extension to store the "night threshold" encoding.  When set to "NO LIGHT", the camera will always take color, no flash images
</commit_message>
<xml_diff>
--- a/tools/spreadsheets/bit-arithmetic.xlsx
+++ b/tools/spreadsheets/bit-arithmetic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\local_repositories\unified-btc-reverse\tools\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE68B285-9A39-4997-83D1-79F27CF65013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C53C5B9-5D86-4A19-8EC2-3F833783A388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24645" yWindow="780" windowWidth="21735" windowHeight="11385" activeTab="1" xr2:uid="{98313939-1963-48D5-BA54-832FAA81C906}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="22515" windowHeight="11385" activeTab="2" xr2:uid="{98313939-1963-48D5-BA54-832FAA81C906}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Shift Left</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Short Bit</t>
   </si>
   <si>
-    <t>Still Snap Exposure</t>
-  </si>
-  <si>
     <t>Unreferenced</t>
   </si>
   <si>
@@ -176,13 +173,25 @@
   </si>
   <si>
     <t>tod_last_photo_in_seconds</t>
+  </si>
+  <si>
+    <t>Sensor Switch</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>BrightnessValue_lo</t>
+  </si>
+  <si>
+    <t>BrightnessValue_hi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,8 +215,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,12 +263,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -319,8 +329,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,19 +342,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -355,14 +362,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D035ACEA-F52A-479E-9F4D-5908A994731D}">
   <dimension ref="A1:BM41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,8 +2342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB2ACC-05C9-4690-926C-F64083D2997B}">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,287 +2359,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C1" s="23">
+      <c r="C1" s="16">
         <v>1</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23">
-        <v>0</v>
-      </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16">
+        <v>0</v>
+      </c>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22">
-        <v>2</v>
-      </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="21">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21">
+        <v>2</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="20">
         <v>1</v>
       </c>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="22">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>15</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>14</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>13</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>12</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>11</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>10</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>9</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <v>8</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="10">
         <v>7</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="10">
         <v>6</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="10">
         <v>5</v>
       </c>
-      <c r="N3" s="12">
-        <v>4</v>
-      </c>
-      <c r="O3" s="12">
+      <c r="N3" s="10">
+        <v>4</v>
+      </c>
+      <c r="O3" s="10">
         <v>3</v>
       </c>
-      <c r="P3" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="12">
+      <c r="P3" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="10">
         <v>1</v>
       </c>
-      <c r="R3" s="12">
-        <v>0</v>
-      </c>
-      <c r="S3" s="11">
+      <c r="R3" s="10">
+        <v>0</v>
+      </c>
+      <c r="S3" s="9">
         <v>15</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="9">
         <v>14</v>
       </c>
-      <c r="U3" s="11">
+      <c r="U3" s="9">
         <v>13</v>
       </c>
-      <c r="V3" s="11">
+      <c r="V3" s="9">
         <v>12</v>
       </c>
-      <c r="W3" s="11">
+      <c r="W3" s="9">
         <v>11</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="9">
         <v>10</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="9">
         <v>9</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Z3" s="9">
         <v>8</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AA3" s="10">
         <v>7</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AB3" s="10">
         <v>6</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="10">
         <v>5</v>
       </c>
-      <c r="AD3" s="12">
-        <v>4</v>
-      </c>
-      <c r="AE3" s="12">
+      <c r="AD3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="10">
         <v>3</v>
       </c>
-      <c r="AF3" s="12">
-        <v>2</v>
-      </c>
-      <c r="AG3" s="12">
+      <c r="AF3" s="10">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="10">
         <v>1</v>
       </c>
-      <c r="AH3" s="12">
+      <c r="AH3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>7</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>6</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>5</v>
       </c>
-      <c r="F4" s="14">
-        <v>4</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="F4" s="12">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12">
         <v>3</v>
       </c>
-      <c r="H4" s="14">
-        <v>2</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="H4" s="12">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="15">
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
         <v>7</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="13">
         <v>6</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="13">
         <v>5</v>
       </c>
-      <c r="N4" s="15">
-        <v>4</v>
-      </c>
-      <c r="O4" s="15">
+      <c r="N4" s="13">
+        <v>4</v>
+      </c>
+      <c r="O4" s="13">
         <v>3</v>
       </c>
-      <c r="P4" s="15">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="15">
+      <c r="P4" s="13">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="13">
         <v>1</v>
       </c>
-      <c r="R4" s="15">
-        <v>0</v>
-      </c>
-      <c r="S4" s="14">
+      <c r="R4" s="13">
+        <v>0</v>
+      </c>
+      <c r="S4" s="12">
         <v>7</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4" s="12">
         <v>6</v>
       </c>
-      <c r="U4" s="14">
+      <c r="U4" s="12">
         <v>5</v>
       </c>
-      <c r="V4" s="14">
-        <v>4</v>
-      </c>
-      <c r="W4" s="14">
+      <c r="V4" s="12">
+        <v>4</v>
+      </c>
+      <c r="W4" s="12">
         <v>3</v>
       </c>
-      <c r="X4" s="14">
-        <v>2</v>
-      </c>
-      <c r="Y4" s="14">
+      <c r="X4" s="12">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="12">
         <v>1</v>
       </c>
-      <c r="Z4" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="15">
+      <c r="Z4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="13">
         <v>7</v>
       </c>
-      <c r="AB4" s="15">
+      <c r="AB4" s="13">
         <v>6</v>
       </c>
-      <c r="AC4" s="15">
+      <c r="AC4" s="13">
         <v>5</v>
       </c>
-      <c r="AD4" s="15">
-        <v>4</v>
-      </c>
-      <c r="AE4" s="15">
+      <c r="AD4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AE4" s="13">
         <v>3</v>
       </c>
-      <c r="AF4" s="15">
-        <v>2</v>
-      </c>
-      <c r="AG4" s="15">
+      <c r="AF4" s="13">
+        <v>2</v>
+      </c>
+      <c r="AG4" s="13">
         <v>1</v>
       </c>
-      <c r="AH4" s="15">
+      <c r="AH4" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2633,37 +2650,47 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
+      <c r="C5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="15"/>
+      <c r="U5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="V5" s="24"/>
+      <c r="W5" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE5" s="27"/>
       <c r="AF5" s="19" t="s">
         <v>33</v>
       </c>
@@ -2681,48 +2708,48 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="20" t="s">
+      <c r="E6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="20"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="23"/>
       <c r="I6" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
-      <c r="O6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
+      <c r="O6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2732,7 +2759,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -2763,8 +2790,8 @@
       <c r="AD7" s="18"/>
       <c r="AE7" s="18"/>
       <c r="AF7" s="18"/>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2773,38 +2800,38 @@
       <c r="B8">
         <v>12</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="26"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2814,7 +2841,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -2923,7 +2950,10 @@
       <c r="AH11" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
     <mergeCell ref="C1:R1"/>
     <mergeCell ref="S1:AH1"/>
     <mergeCell ref="C5:R5"/>
@@ -2939,6 +2969,7 @@
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="U5:V5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Foundational Bug Fixed -- Rev 2023-09-14
Major bug fixes to updated function across all camera types.  Included fixes to Bug1 and Bug2 in the database.  (Pressure/temperature reading on BTC-8E -- SpecOps Edge; and Day/Night threshold).  Ohers.
</commit_message>
<xml_diff>
--- a/tools/spreadsheets/bit-arithmetic.xlsx
+++ b/tools/spreadsheets/bit-arithmetic.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\local_repositories\unified-btc-reverse\tools\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C53C5B9-5D86-4A19-8EC2-3F833783A388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F130B91-DBC7-4522-A3C4-0F309CFEF130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="22515" windowHeight="11385" activeTab="2" xr2:uid="{98313939-1963-48D5-BA54-832FAA81C906}"/>
+    <workbookView xWindow="25920" yWindow="2385" windowWidth="24750" windowHeight="9795" activeTab="2" xr2:uid="{98313939-1963-48D5-BA54-832FAA81C906}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BTC-78E" sheetId="4" r:id="rId3"/>
+    <sheet name="BTC-78E-HP4" sheetId="5" r:id="rId4"/>
+    <sheet name="BTC-78E-HP5" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$J$22</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Shift Left</t>
   </si>
@@ -185,6 +187,15 @@
   </si>
   <si>
     <t>BrightnessValue_hi</t>
+  </si>
+  <si>
+    <t>aperture</t>
+  </si>
+  <si>
+    <t>operation_mode</t>
+  </si>
+  <si>
+    <t>used</t>
   </si>
 </sst>
 </file>
@@ -223,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +295,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -315,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -342,8 +359,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,9 +395,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -368,16 +409,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2339,550 +2374,561 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB2ACC-05C9-4690-926C-F64083D2997B}">
-  <dimension ref="A1:AH11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4653FA9-4DE7-44AA-85D7-DF201EF59258}">
+  <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:AF7"/>
+      <selection activeCell="D7" sqref="D7:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="18" width="6" customWidth="1"/>
-    <col min="19" max="26" width="5.85546875" customWidth="1"/>
-    <col min="27" max="34" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="19" width="6" customWidth="1"/>
+    <col min="20" max="27" width="5.85546875" customWidth="1"/>
+    <col min="28" max="35" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C1" s="16">
-        <v>1</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16">
-        <v>0</v>
-      </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D1" s="25">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25">
+        <v>0</v>
+      </c>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20">
+      <c r="D2" s="28">
         <v>3</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21">
-        <v>2</v>
-      </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="20">
-        <v>1</v>
-      </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="21">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29">
+        <v>2</v>
+      </c>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28">
+        <v>1</v>
+      </c>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="29">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="9">
+      <c r="D3" s="9">
         <v>15</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="9">
         <v>14</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="9">
         <v>13</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
         <v>12</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="9">
         <v>11</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="9">
         <v>10</v>
       </c>
-      <c r="I3" s="9">
+      <c r="J3" s="9">
         <v>9</v>
       </c>
-      <c r="J3" s="9">
+      <c r="K3" s="9">
         <v>8</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="10">
         <v>7</v>
       </c>
-      <c r="L3" s="10">
+      <c r="M3" s="10">
         <v>6</v>
       </c>
-      <c r="M3" s="10">
+      <c r="N3" s="10">
         <v>5</v>
       </c>
-      <c r="N3" s="10">
-        <v>4</v>
-      </c>
       <c r="O3" s="10">
+        <v>4</v>
+      </c>
+      <c r="P3" s="10">
         <v>3</v>
       </c>
-      <c r="P3" s="10">
-        <v>2</v>
-      </c>
       <c r="Q3" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" s="10">
-        <v>0</v>
-      </c>
-      <c r="S3" s="9">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0</v>
+      </c>
+      <c r="T3" s="9">
         <v>15</v>
       </c>
-      <c r="T3" s="9">
+      <c r="U3" s="9">
         <v>14</v>
       </c>
-      <c r="U3" s="9">
+      <c r="V3" s="9">
         <v>13</v>
       </c>
-      <c r="V3" s="9">
+      <c r="W3" s="9">
         <v>12</v>
       </c>
-      <c r="W3" s="9">
+      <c r="X3" s="9">
         <v>11</v>
       </c>
-      <c r="X3" s="9">
+      <c r="Y3" s="9">
         <v>10</v>
       </c>
-      <c r="Y3" s="9">
+      <c r="Z3" s="9">
         <v>9</v>
       </c>
-      <c r="Z3" s="9">
+      <c r="AA3" s="9">
         <v>8</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AB3" s="10">
         <v>7</v>
       </c>
-      <c r="AB3" s="10">
+      <c r="AC3" s="10">
         <v>6</v>
       </c>
-      <c r="AC3" s="10">
+      <c r="AD3" s="10">
         <v>5</v>
       </c>
-      <c r="AD3" s="10">
-        <v>4</v>
-      </c>
       <c r="AE3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="10">
         <v>3</v>
       </c>
-      <c r="AF3" s="10">
-        <v>2</v>
-      </c>
       <c r="AG3" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="12">
+      <c r="D4" s="12">
         <v>7</v>
       </c>
-      <c r="D4" s="12">
+      <c r="E4" s="12">
         <v>6</v>
       </c>
-      <c r="E4" s="12">
+      <c r="F4" s="12">
         <v>5</v>
       </c>
-      <c r="F4" s="12">
-        <v>4</v>
-      </c>
       <c r="G4" s="12">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12">
         <v>3</v>
       </c>
-      <c r="H4" s="12">
-        <v>2</v>
-      </c>
       <c r="I4" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="12">
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
         <v>7</v>
       </c>
-      <c r="L4" s="13">
+      <c r="M4" s="13">
         <v>6</v>
       </c>
-      <c r="M4" s="13">
+      <c r="N4" s="13">
         <v>5</v>
       </c>
-      <c r="N4" s="13">
-        <v>4</v>
-      </c>
       <c r="O4" s="13">
+        <v>4</v>
+      </c>
+      <c r="P4" s="13">
         <v>3</v>
       </c>
-      <c r="P4" s="13">
-        <v>2</v>
-      </c>
       <c r="Q4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" s="13">
-        <v>0</v>
-      </c>
-      <c r="S4" s="12">
+        <v>1</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="12">
         <v>7</v>
       </c>
-      <c r="T4" s="12">
+      <c r="U4" s="12">
         <v>6</v>
       </c>
-      <c r="U4" s="12">
+      <c r="V4" s="12">
         <v>5</v>
       </c>
-      <c r="V4" s="12">
-        <v>4</v>
-      </c>
       <c r="W4" s="12">
+        <v>4</v>
+      </c>
+      <c r="X4" s="12">
         <v>3</v>
       </c>
-      <c r="X4" s="12">
-        <v>2</v>
-      </c>
       <c r="Y4" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="13">
         <v>7</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AC4" s="13">
         <v>6</v>
       </c>
-      <c r="AC4" s="13">
+      <c r="AD4" s="13">
         <v>5</v>
       </c>
-      <c r="AD4" s="13">
-        <v>4</v>
-      </c>
       <c r="AE4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="13">
         <v>3</v>
       </c>
-      <c r="AF4" s="13">
-        <v>2</v>
-      </c>
       <c r="AG4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="15" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="15"/>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="17"/>
+      <c r="V5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="V5" s="24"/>
-      <c r="W5" s="25" t="s">
+      <c r="W5" s="19"/>
+      <c r="X5" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="24" t="s">
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="26" t="s">
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="19" t="s">
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="8" t="s">
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="8"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="19" t="s">
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="19"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
         <v>8</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>12</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+      <c r="AG8" s="17"/>
+      <c r="AH8" s="17"/>
+      <c r="AI8" s="17"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>16</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-      <c r="AH9" s="19"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2890,7 +2936,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="7"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -2898,7 +2944,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="4"/>
+      <c r="S10" s="7"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -2906,7 +2952,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
-      <c r="AA10" s="7"/>
+      <c r="AA10" s="4"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -2914,9 +2960,18 @@
       <c r="AF10" s="7"/>
       <c r="AG10" s="7"/>
       <c r="AH10" s="7"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
+      <c r="AI10" s="7"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2924,7 +2979,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="7"/>
+      <c r="K11" s="4"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -2932,7 +2987,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
-      <c r="S11" s="4"/>
+      <c r="S11" s="7"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
@@ -2940,7 +2995,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AA11" s="7"/>
+      <c r="AA11" s="4"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -2948,28 +3003,1363 @@
       <c r="AF11" s="7"/>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="D7:AG7"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="L6:S6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="T6:AI6"/>
+    <mergeCell ref="D5:S5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="D1:S1"/>
+    <mergeCell ref="T1:AI1"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="L2:S2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="AB2:AI2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39993D64-337B-4B51-988E-D512978217BD}">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="19" width="6" customWidth="1"/>
+    <col min="20" max="27" width="5.85546875" customWidth="1"/>
+    <col min="28" max="35" width="6.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D1" s="25">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25">
+        <v>0</v>
+      </c>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="28">
+        <v>3</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29">
+        <v>2</v>
+      </c>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28">
+        <v>1</v>
+      </c>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="29">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9">
+        <v>14</v>
+      </c>
+      <c r="F3" s="9">
+        <v>13</v>
+      </c>
+      <c r="G3" s="9">
+        <v>12</v>
+      </c>
+      <c r="H3" s="9">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>10</v>
+      </c>
+      <c r="J3" s="9">
+        <v>9</v>
+      </c>
+      <c r="K3" s="9">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10">
+        <v>7</v>
+      </c>
+      <c r="M3" s="10">
+        <v>6</v>
+      </c>
+      <c r="N3" s="10">
+        <v>5</v>
+      </c>
+      <c r="O3" s="10">
+        <v>4</v>
+      </c>
+      <c r="P3" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2</v>
+      </c>
+      <c r="R3" s="10">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0</v>
+      </c>
+      <c r="T3" s="9">
+        <v>15</v>
+      </c>
+      <c r="U3" s="9">
+        <v>14</v>
+      </c>
+      <c r="V3" s="9">
+        <v>13</v>
+      </c>
+      <c r="W3" s="9">
+        <v>12</v>
+      </c>
+      <c r="X3" s="9">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>7</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>6</v>
+      </c>
+      <c r="AD3" s="10">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="12">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12">
+        <v>6</v>
+      </c>
+      <c r="F4" s="12">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>7</v>
+      </c>
+      <c r="M4" s="13">
+        <v>6</v>
+      </c>
+      <c r="N4" s="13">
+        <v>5</v>
+      </c>
+      <c r="O4" s="13">
+        <v>4</v>
+      </c>
+      <c r="P4" s="13">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>2</v>
+      </c>
+      <c r="R4" s="13">
+        <v>1</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="12">
+        <v>7</v>
+      </c>
+      <c r="U4" s="12">
+        <v>6</v>
+      </c>
+      <c r="V4" s="12">
+        <v>5</v>
+      </c>
+      <c r="W4" s="12">
+        <v>4</v>
+      </c>
+      <c r="X4" s="12">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="13">
+        <v>6</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="13">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="17"/>
+      <c r="V5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="19"/>
+      <c r="X5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="31"/>
+      <c r="J6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="22"/>
+      <c r="L6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+      <c r="AG8" s="17"/>
+      <c r="AH8" s="17"/>
+      <c r="AI8" s="17"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="D7:AG7"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="T6:AI6"/>
+    <mergeCell ref="D5:S5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="D1:S1"/>
+    <mergeCell ref="T1:AI1"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="L2:S2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="AB2:AI2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB2ACC-05C9-4690-926C-F64083D2997B}">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5:AD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="19" width="6" customWidth="1"/>
+    <col min="20" max="27" width="5.85546875" customWidth="1"/>
+    <col min="28" max="35" width="6.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D1" s="25">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25">
+        <v>0</v>
+      </c>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="28">
+        <v>3</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29">
+        <v>2</v>
+      </c>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28">
+        <v>1</v>
+      </c>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="29">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9">
+        <v>14</v>
+      </c>
+      <c r="F3" s="9">
+        <v>13</v>
+      </c>
+      <c r="G3" s="9">
+        <v>12</v>
+      </c>
+      <c r="H3" s="9">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>10</v>
+      </c>
+      <c r="J3" s="9">
+        <v>9</v>
+      </c>
+      <c r="K3" s="9">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10">
+        <v>7</v>
+      </c>
+      <c r="M3" s="10">
+        <v>6</v>
+      </c>
+      <c r="N3" s="10">
+        <v>5</v>
+      </c>
+      <c r="O3" s="10">
+        <v>4</v>
+      </c>
+      <c r="P3" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2</v>
+      </c>
+      <c r="R3" s="10">
+        <v>1</v>
+      </c>
+      <c r="S3" s="10">
+        <v>0</v>
+      </c>
+      <c r="T3" s="9">
+        <v>15</v>
+      </c>
+      <c r="U3" s="9">
+        <v>14</v>
+      </c>
+      <c r="V3" s="9">
+        <v>13</v>
+      </c>
+      <c r="W3" s="9">
+        <v>12</v>
+      </c>
+      <c r="X3" s="9">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>7</v>
+      </c>
+      <c r="AC3" s="10">
+        <v>6</v>
+      </c>
+      <c r="AD3" s="10">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="10">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="10">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="12">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12">
+        <v>6</v>
+      </c>
+      <c r="F4" s="12">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>7</v>
+      </c>
+      <c r="M4" s="13">
+        <v>6</v>
+      </c>
+      <c r="N4" s="13">
+        <v>5</v>
+      </c>
+      <c r="O4" s="13">
+        <v>4</v>
+      </c>
+      <c r="P4" s="13">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>2</v>
+      </c>
+      <c r="R4" s="13">
+        <v>1</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+      <c r="T4" s="12">
+        <v>7</v>
+      </c>
+      <c r="U4" s="12">
+        <v>6</v>
+      </c>
+      <c r="V4" s="12">
+        <v>5</v>
+      </c>
+      <c r="W4" s="12">
+        <v>4</v>
+      </c>
+      <c r="X4" s="12">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="13">
+        <v>6</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="13">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="13">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="17"/>
+      <c r="V5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="19"/>
+      <c r="X5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI5" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="31"/>
+      <c r="J6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="22"/>
+      <c r="L6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+      <c r="AG8" s="17"/>
+      <c r="AH8" s="17"/>
+      <c r="AI8" s="17"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="C1:R1"/>
-    <mergeCell ref="S1:AH1"/>
-    <mergeCell ref="C5:R5"/>
-    <mergeCell ref="C7:AF7"/>
-    <mergeCell ref="C9:AH9"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="S2:Z2"/>
-    <mergeCell ref="AA2:AH2"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="S6:AH6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="D1:S1"/>
+    <mergeCell ref="T1:AI1"/>
+    <mergeCell ref="D5:S5"/>
+    <mergeCell ref="D7:AG7"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="L2:S2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="AB2:AI2"/>
+    <mergeCell ref="T6:AI6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="D9:AE9"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>